<commit_message>
nuevo array de productos
</commit_message>
<xml_diff>
--- a/src/data/tienda360.xlsx
+++ b/src/data/tienda360.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmatiasm/Documents/MATIAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmatiasm/Documents/MATIAS/PROYECTO-MATIAS/Calin_Repositorio_Mocks/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C64961-DD19-974A-B2CE-2D963DDA3F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377F766-25C0-D14C-BEB4-D81137FA450F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{A60726CA-E045-3D44-984C-DD3A0D447AE4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>imagen de gaseosa</t>
+  </si>
+  <si>
+    <t>vicio</t>
+  </si>
+  <si>
+    <t>imagen de producto</t>
   </si>
 </sst>
 </file>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1018D657-1B63-1F42-8956-31EDCD85751D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,6 +574,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>1.3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>